<commit_message>
feat: fill datasheet content
</commit_message>
<xml_diff>
--- a/template/data-worksheet.xlsx
+++ b/template/data-worksheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF90F21-C421-4D85-8A25-979741064EC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58ECE8BB-37F6-43EA-843B-56031C2FF24B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +12,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Техника!$1:$6</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Техника!$A$1:$K$133</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Техника!$A$1:$K$156</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="50">
   <si>
     <t>Версия программы: 1.0.0</t>
   </si>
@@ -153,9 +153,6 @@
   </si>
   <si>
     <t>d, мм</t>
-  </si>
-  <si>
-    <t>e, мм</t>
   </si>
   <si>
     <t>D1, мм</t>
@@ -257,7 +254,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF1769C3"/>
+        <fgColor theme="4" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -274,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -319,16 +316,46 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -338,32 +365,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -395,7 +413,7 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>323850</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>49530</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -433,7 +451,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>170794</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>151087</xdr:rowOff>
+      <xdr:rowOff>105367</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
@@ -468,8 +486,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="171450" y="552450"/>
-          <a:ext cx="1781175" cy="571500"/>
+          <a:off x="170794" y="501607"/>
+          <a:ext cx="1782816" cy="563098"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -489,7 +507,7 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>17145</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -788,10 +806,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K132"/>
+  <dimension ref="A1:K131"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A56" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I126" sqref="I126"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A122" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E136" sqref="E136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -799,40 +817,40 @@
     <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="28"/>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-    </row>
-    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+    <row r="1" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="40"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+    </row>
+    <row r="2" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-    </row>
-    <row r="3" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+    </row>
+    <row r="3" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="5"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
       <c r="G3" s="8"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+    </row>
+    <row r="4" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C4" s="11"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="H4" s="24" t="s">
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="H4" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="24"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-    </row>
-    <row r="5" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I4" s="34"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+    </row>
+    <row r="5" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
       <c r="C5" s="13"/>
@@ -844,10 +862,10 @@
         <v>1</v>
       </c>
       <c r="I5" s="3"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-    </row>
-    <row r="6" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+    </row>
+    <row r="6" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="7"/>
@@ -860,22 +878,22 @@
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="22" t="s">
+    <row r="7" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-    </row>
-    <row r="8" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+    </row>
+    <row r="8" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -887,14 +905,14 @@
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
     </row>
-    <row r="9" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="24" t="s">
+    <row r="9" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14" t="s">
         <v>30</v>
@@ -903,14 +921,14 @@
       <c r="J9" s="2"/>
       <c r="K9" s="15"/>
     </row>
-    <row r="10" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="24" t="s">
+    <row r="10" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14" t="s">
         <v>31</v>
@@ -919,14 +937,14 @@
       <c r="J10" s="2"/>
       <c r="K10" s="15"/>
     </row>
-    <row r="11" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="24" t="s">
+    <row r="11" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
       <c r="G11" s="14"/>
       <c r="H11" s="14" t="s">
         <v>32</v>
@@ -935,75 +953,79 @@
       <c r="J11" s="2"/>
       <c r="K11" s="15"/>
     </row>
-    <row r="12" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="24" t="s">
+    <row r="12" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14" t="s">
         <v>34</v>
       </c>
       <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
+      <c r="J12" s="26">
+        <f>G24+H68+H80+H92+H104+H116+H128</f>
+        <v>0</v>
+      </c>
       <c r="K12" s="15"/>
     </row>
-    <row r="14" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="21" t="s">
+    <row r="13" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-    </row>
-    <row r="15" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B16" s="25" t="s">
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
+    </row>
+    <row r="15" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="27" t="s">
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="25" t="s">
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+    </row>
+    <row r="17" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="27" t="s">
+      <c r="F17" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="27"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="25" t="s">
+      <c r="G17" s="29"/>
+    </row>
+    <row r="18" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="26" t="s">
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-    </row>
-    <row r="19" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+    </row>
+    <row r="19" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
         <v>21</v>
       </c>
@@ -1011,7 +1033,7 @@
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
         <v>11</v>
       </c>
@@ -1019,7 +1041,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
         <v>12</v>
       </c>
@@ -1027,7 +1049,7 @@
       <c r="F21" s="17"/>
       <c r="G21" s="17"/>
     </row>
-    <row r="22" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
         <v>13</v>
       </c>
@@ -1035,7 +1057,7 @@
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
     </row>
-    <row r="23" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
         <v>20</v>
       </c>
@@ -1043,25 +1065,50 @@
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
     </row>
-    <row r="24" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
         <v>33</v>
       </c>
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-    </row>
-    <row r="25" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G24" s="25"/>
+    </row>
+    <row r="25" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="16"/>
     </row>
-    <row r="41" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="10" t="s">
         <v>15</v>
       </c>
@@ -1081,262 +1128,310 @@
         <v>19</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="18"/>
-      <c r="C55" s="18"/>
-      <c r="D55" s="18"/>
-      <c r="E55" s="18"/>
-      <c r="F55" s="18"/>
-      <c r="G55" s="18"/>
-    </row>
-    <row r="58" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="21" t="s">
+    <row r="55" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="23"/>
+      <c r="C55" s="23"/>
+      <c r="D55" s="23"/>
+      <c r="E55" s="23"/>
+      <c r="F55" s="24"/>
+      <c r="G55" s="23"/>
+    </row>
+    <row r="56" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B58" s="21"/>
-      <c r="C58" s="21"/>
-      <c r="D58" s="21"/>
-      <c r="E58" s="21"/>
-      <c r="F58" s="21"/>
-      <c r="G58" s="21"/>
-      <c r="H58" s="21"/>
-      <c r="I58" s="21"/>
-      <c r="J58" s="21"/>
-      <c r="K58" s="21"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B60" t="s">
+      <c r="B56" s="31"/>
+      <c r="C56" s="31"/>
+      <c r="D56" s="31"/>
+      <c r="E56" s="31"/>
+      <c r="F56" s="31"/>
+      <c r="G56" s="31"/>
+      <c r="H56" s="31"/>
+      <c r="I56" s="31"/>
+      <c r="J56" s="31"/>
+      <c r="K56" s="31"/>
+    </row>
+    <row r="57" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B69" s="10" t="s">
+    <row r="59" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="63" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="65" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="66" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="67" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C69" s="10" t="s">
+      <c r="C67" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D69" s="10" t="s">
+      <c r="D67" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E69" s="10" t="s">
+      <c r="E67" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F69" s="10" t="s">
+      <c r="F67" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="G69" s="10" t="s">
+      <c r="G67" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="H69" s="10" t="s">
+      <c r="H67" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B70" s="10"/>
-      <c r="C70" s="10"/>
-      <c r="D70" s="10"/>
-      <c r="E70" s="10"/>
-      <c r="F70" s="10"/>
-      <c r="G70" s="10"/>
-      <c r="H70" s="10"/>
-    </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B72" t="s">
+    <row r="68" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="21"/>
+      <c r="C68" s="21"/>
+      <c r="D68" s="22"/>
+      <c r="E68" s="21"/>
+      <c r="F68" s="21"/>
+      <c r="G68" s="21"/>
+      <c r="H68" s="21"/>
+    </row>
+    <row r="69" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="70" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="72" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="73" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="74" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="75" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="76" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="77" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="78" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="79" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B79" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C79" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D79" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E79" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F79" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G79" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H79" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B80" s="21"/>
+      <c r="C80" s="21"/>
+      <c r="D80" s="22"/>
+      <c r="E80" s="21"/>
+      <c r="F80" s="21"/>
+      <c r="G80" s="21"/>
+      <c r="H80" s="21"/>
+    </row>
+    <row r="81" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="82" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B82" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B81" s="10" t="s">
+    <row r="83" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="84" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="85" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="86" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="87" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="88" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="89" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="90" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="91" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B91" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C81" s="10" t="s">
+      <c r="C91" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D81" s="10" t="s">
+      <c r="D91" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E81" s="10" t="s">
+      <c r="E91" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F81" s="10" t="s">
+      <c r="F91" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="G81" s="10" t="s">
+      <c r="G91" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="H81" s="10" t="s">
+      <c r="H91" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B82" s="10"/>
-      <c r="C82" s="10"/>
-      <c r="D82" s="10"/>
-      <c r="E82" s="10"/>
-      <c r="F82" s="10"/>
-      <c r="G82" s="10"/>
-      <c r="H82" s="10"/>
-    </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B84" t="s">
+    <row r="92" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B92" s="21"/>
+      <c r="C92" s="21"/>
+      <c r="D92" s="22"/>
+      <c r="E92" s="21"/>
+      <c r="F92" s="21"/>
+      <c r="G92" s="21"/>
+      <c r="H92" s="21"/>
+    </row>
+    <row r="93" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="94" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B94" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="95" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="96" spans="2:8" s="19" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="97" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="98" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="99" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="100" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="101" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="102" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="103" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B103" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C103" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D103" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E103" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F103" s="18"/>
+      <c r="G103" s="18"/>
+      <c r="H103" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="104" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B104" s="20"/>
+      <c r="C104" s="20"/>
+      <c r="D104" s="20"/>
+      <c r="E104" s="20"/>
+      <c r="F104" s="20"/>
+      <c r="G104" s="20"/>
+      <c r="H104" s="20"/>
+    </row>
+    <row r="105" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="106" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B106" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="107" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="108" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="109" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="110" spans="2:8" s="19" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="111" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="112" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="113" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="114" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="115" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B115" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C115" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D115" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E115" s="10"/>
+      <c r="F115" s="10"/>
+      <c r="G115" s="10"/>
+      <c r="H115" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="116" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B116" s="21"/>
+      <c r="C116" s="21"/>
+      <c r="D116" s="21"/>
+      <c r="E116" s="21"/>
+      <c r="F116" s="21"/>
+      <c r="G116" s="21"/>
+      <c r="H116" s="21"/>
+    </row>
+    <row r="117" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="118" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B118" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="119" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="120" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="121" spans="2:8" s="19" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="122" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="123" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="124" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="125" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="126" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="127" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B127" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C127" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D127" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E127" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="F127" s="18"/>
+      <c r="G127" s="18"/>
+      <c r="H127" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="128" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B128" s="20"/>
+      <c r="C128" s="20"/>
+      <c r="D128" s="20"/>
+      <c r="E128" s="20"/>
+      <c r="F128" s="20"/>
+      <c r="G128" s="20"/>
+      <c r="H128" s="20"/>
+    </row>
+    <row r="129" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="130" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="27" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B93" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C93" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D93" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E93" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F93" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G93" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="H93" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="94" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B94" s="10"/>
-      <c r="C94" s="10"/>
-      <c r="D94" s="10"/>
-      <c r="E94" s="10"/>
-      <c r="F94" s="10"/>
-      <c r="G94" s="10"/>
-      <c r="H94" s="10"/>
-    </row>
-    <row r="96" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="97" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="98" spans="2:8" s="20" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="99" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="100" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="101" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="102" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="103" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="104" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="105" spans="2:8" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B105" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C105" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="D105" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E105" s="19"/>
-      <c r="F105" s="19"/>
-      <c r="G105" s="19"/>
-      <c r="H105" s="19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="106" spans="2:8" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="19"/>
-      <c r="C106" s="19"/>
-      <c r="D106" s="19"/>
-      <c r="E106" s="19"/>
-      <c r="F106" s="19"/>
-      <c r="G106" s="19"/>
-      <c r="H106" s="19"/>
-    </row>
-    <row r="107" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="108" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B108" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="112" spans="2:8" s="20" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="117" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B117" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C117" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D117" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E117" s="10"/>
-      <c r="F117" s="10"/>
-      <c r="G117" s="10"/>
-      <c r="H117" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="118" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B118" s="10"/>
-      <c r="C118" s="10"/>
-      <c r="D118" s="10"/>
-      <c r="E118" s="10"/>
-      <c r="F118" s="10"/>
-      <c r="G118" s="10"/>
-      <c r="H118" s="10"/>
-    </row>
-    <row r="120" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B120" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="123" spans="2:8" s="20" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="129" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B129" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="C129" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="D129" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E129" s="19"/>
-      <c r="F129" s="19"/>
-      <c r="G129" s="19"/>
-      <c r="H129" s="19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="130" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B130" s="19"/>
-      <c r="C130" s="19"/>
-      <c r="D130" s="19"/>
-      <c r="E130" s="19"/>
-      <c r="F130" s="19"/>
-      <c r="G130" s="19"/>
-      <c r="H130" s="19"/>
-    </row>
-    <row r="132" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A132" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="B132" s="21"/>
-      <c r="C132" s="21"/>
-      <c r="D132" s="21"/>
-      <c r="E132" s="21"/>
-      <c r="F132" s="21"/>
-      <c r="G132" s="21"/>
-      <c r="H132" s="21"/>
-      <c r="I132" s="21"/>
-      <c r="J132" s="21"/>
-      <c r="K132" s="21"/>
-    </row>
+      <c r="B130" s="27"/>
+      <c r="C130" s="27"/>
+      <c r="D130" s="27"/>
+      <c r="E130" s="27"/>
+      <c r="F130" s="27"/>
+      <c r="G130" s="27"/>
+      <c r="H130" s="27"/>
+      <c r="I130" s="27"/>
+      <c r="J130" s="27"/>
+      <c r="K130" s="27"/>
+    </row>
+    <row r="131" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="A132:K132"/>
+  <mergeCells count="26">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="B9:D9"/>
@@ -1351,7 +1446,7 @@
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="E16:G16"/>
     <mergeCell ref="B16:D16"/>
-    <mergeCell ref="A58:K58"/>
+    <mergeCell ref="A56:K56"/>
     <mergeCell ref="A7:K7"/>
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="E11:F11"/>

</xml_diff>

<commit_message>
feat: add calculate total weigth and project name to datasheet
</commit_message>
<xml_diff>
--- a/template/data-worksheet.xlsx
+++ b/template/data-worksheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58ECE8BB-37F6-43EA-843B-56031C2FF24B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D46313A-B7F4-452A-BB72-6AF279AE060A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -344,6 +344,24 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -362,26 +380,8 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -808,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K131"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A122" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E136" sqref="E136"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -818,37 +818,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="40"/>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
+      <c r="A1" s="28"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
     </row>
     <row r="2" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
     </row>
     <row r="3" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="5"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
       <c r="G3" s="8"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
     </row>
     <row r="4" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C4" s="11"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="H4" s="34" t="s">
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="H4" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="34"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
     </row>
     <row r="5" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
@@ -862,8 +862,8 @@
         <v>1</v>
       </c>
       <c r="I5" s="3"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
     </row>
     <row r="6" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
@@ -879,19 +879,19 @@
       <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
     </row>
     <row r="8" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="9"/>
@@ -906,13 +906,13 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14" t="s">
         <v>30</v>
@@ -922,13 +922,13 @@
       <c r="K9" s="15"/>
     </row>
     <row r="10" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14" t="s">
         <v>31</v>
@@ -938,13 +938,13 @@
       <c r="K10" s="15"/>
     </row>
     <row r="11" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="14"/>
       <c r="H11" s="14" t="s">
         <v>32</v>
@@ -954,76 +954,73 @@
       <c r="K11" s="15"/>
     </row>
     <row r="12" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14" t="s">
         <v>34</v>
       </c>
       <c r="I12" s="2"/>
-      <c r="J12" s="26">
-        <f>G24+H68+H80+H92+H104+H116+H128</f>
-        <v>0</v>
-      </c>
+      <c r="J12" s="26"/>
       <c r="K12" s="15"/>
     </row>
     <row r="13" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="37"/>
     </row>
     <row r="15" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="29" t="s">
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
     </row>
     <row r="17" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="29" t="s">
+      <c r="F17" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="29"/>
+      <c r="G17" s="35"/>
     </row>
     <row r="18" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="35" t="s">
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
     </row>
     <row r="19" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
@@ -1137,19 +1134,19 @@
       <c r="G55" s="23"/>
     </row>
     <row r="56" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="31" t="s">
+      <c r="A56" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B56" s="31"/>
-      <c r="C56" s="31"/>
-      <c r="D56" s="31"/>
-      <c r="E56" s="31"/>
-      <c r="F56" s="31"/>
-      <c r="G56" s="31"/>
-      <c r="H56" s="31"/>
-      <c r="I56" s="31"/>
-      <c r="J56" s="31"/>
-      <c r="K56" s="31"/>
+      <c r="B56" s="37"/>
+      <c r="C56" s="37"/>
+      <c r="D56" s="37"/>
+      <c r="E56" s="37"/>
+      <c r="F56" s="37"/>
+      <c r="G56" s="37"/>
+      <c r="H56" s="37"/>
+      <c r="I56" s="37"/>
+      <c r="J56" s="37"/>
+      <c r="K56" s="37"/>
     </row>
     <row r="57" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -1432,17 +1429,6 @@
     <row r="131" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="E16:G16"/>
     <mergeCell ref="B16:D16"/>
@@ -1458,6 +1444,17 @@
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="A14:K14"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="7.874015748031496E-2" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.19685039370078741"/>

</xml_diff>

<commit_message>
feat: add convert to pdf with libre, edit datasheet with typo and add page breakes
</commit_message>
<xml_diff>
--- a/template/data-worksheet.xlsx
+++ b/template/data-worksheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D46313A-B7F4-452A-BB72-6AF279AE060A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89FD5549-4D50-4241-96DA-214621A374BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -113,9 +113,6 @@
     <t>Система:</t>
   </si>
   <si>
-    <t>Наиментование модели:</t>
-  </si>
-  <si>
     <t>Ширина, мм:</t>
   </si>
   <si>
@@ -174,6 +171,9 @@
   </si>
   <si>
     <t>Схемы</t>
+  </si>
+  <si>
+    <t>Наименование модели:</t>
   </si>
 </sst>
 </file>
@@ -808,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K131"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A149" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E163" sqref="E163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -915,7 +915,7 @@
       <c r="F9" s="39"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -931,7 +931,7 @@
       <c r="F10" s="39"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -947,7 +947,7 @@
       <c r="F11" s="39"/>
       <c r="G11" s="14"/>
       <c r="H11" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -955,7 +955,7 @@
     </row>
     <row r="12" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="29" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="C12" s="29"/>
       <c r="D12" s="29"/>
@@ -963,7 +963,7 @@
       <c r="F12" s="39"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="26"/>
@@ -1064,7 +1064,7 @@
     </row>
     <row r="24" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
@@ -1116,7 +1116,7 @@
         <v>17</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F54" s="10" t="s">
         <v>18</v>
@@ -1164,25 +1164,25 @@
     <row r="66" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="67" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B67" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C67" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C67" s="10" t="s">
+      <c r="D67" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D67" s="10" t="s">
+      <c r="E67" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E67" s="10" t="s">
+      <c r="F67" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F67" s="10" t="s">
+      <c r="G67" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H67" s="10" t="s">
         <v>40</v>
-      </c>
-      <c r="G67" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="H67" s="10" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="68" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -1197,7 +1197,7 @@
     <row r="69" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="70" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="71" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1210,25 +1210,25 @@
     <row r="78" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="79" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B79" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C79" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C79" s="10" t="s">
+      <c r="D79" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D79" s="10" t="s">
+      <c r="E79" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E79" s="10" t="s">
+      <c r="F79" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F79" s="10" t="s">
+      <c r="G79" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H79" s="10" t="s">
         <v>40</v>
-      </c>
-      <c r="G79" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="H79" s="10" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="80" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -1243,7 +1243,7 @@
     <row r="81" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="82" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="83" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1256,25 +1256,25 @@
     <row r="90" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="91" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B91" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C91" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C91" s="10" t="s">
+      <c r="D91" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D91" s="10" t="s">
+      <c r="E91" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E91" s="10" t="s">
+      <c r="F91" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F91" s="10" t="s">
+      <c r="G91" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H91" s="10" t="s">
         <v>40</v>
-      </c>
-      <c r="G91" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="H91" s="10" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="92" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -1302,13 +1302,13 @@
     <row r="102" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="103" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B103" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C103" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C103" s="18" t="s">
-        <v>44</v>
-      </c>
       <c r="D103" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E103" s="18" t="s">
         <v>15</v>
@@ -1316,7 +1316,7 @@
       <c r="F103" s="18"/>
       <c r="G103" s="18"/>
       <c r="H103" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="104" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -1344,19 +1344,19 @@
     <row r="114" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="115" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B115" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C115" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D115" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E115" s="10"/>
       <c r="F115" s="10"/>
       <c r="G115" s="10"/>
       <c r="H115" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="116" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -1371,7 +1371,7 @@
     <row r="117" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="118" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B118" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="119" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1384,21 +1384,21 @@
     <row r="126" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="127" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B127" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C127" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D127" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E127" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F127" s="18"/>
       <c r="G127" s="18"/>
       <c r="H127" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="128" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -1413,7 +1413,7 @@
     <row r="129" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="130" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B130" s="27"/>
       <c r="C130" s="27"/>

</xml_diff>

<commit_message>
feat: replace 2,25 fan with 2,2, add env variable for dev mode, fix date and weight in data sheet
</commit_message>
<xml_diff>
--- a/template/data-worksheet.xlsx
+++ b/template/data-worksheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89FD5549-4D50-4241-96DA-214621A374BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E9F444-21C6-4BD6-93D9-F5D4F0DA42D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -86,9 +86,6 @@
     <t>L3, мм</t>
   </si>
   <si>
-    <t>Уровень звуковой мощности вход/выход, дБ(А):</t>
-  </si>
-  <si>
     <t>Электропитание, В / ф:</t>
   </si>
   <si>
@@ -174,6 +171,9 @@
   </si>
   <si>
     <t>Наименование модели:</t>
+  </si>
+  <si>
+    <t>Уровень звуковой мощности, дБ(А):</t>
   </si>
 </sst>
 </file>
@@ -344,44 +344,44 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -808,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K131"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A149" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E163" sqref="E163"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A6" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -818,37 +818,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="28"/>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
+      <c r="A1" s="40"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
     </row>
     <row r="2" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
     </row>
     <row r="3" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="5"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
       <c r="G3" s="8"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
     </row>
     <row r="4" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C4" s="11"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="H4" s="29" t="s">
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="H4" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="29"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="31"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
     </row>
     <row r="5" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
@@ -862,8 +862,8 @@
         <v>1</v>
       </c>
       <c r="I5" s="3"/>
-      <c r="J5" s="34"/>
-      <c r="K5" s="34"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
     </row>
     <row r="6" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
@@ -879,19 +879,19 @@
       <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
     </row>
     <row r="8" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="9"/>
@@ -906,64 +906,64 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
+      <c r="B9" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="15"/>
     </row>
     <row r="10" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
+      <c r="B10" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="15"/>
     </row>
     <row r="11" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="B11" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
       <c r="G11" s="14"/>
       <c r="H11" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="15"/>
     </row>
     <row r="12" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
+      <c r="B12" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="26"/>
@@ -971,60 +971,60 @@
     </row>
     <row r="13" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="37"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
     </row>
     <row r="15" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="35" t="s">
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
     </row>
     <row r="17" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="35" t="s">
+      <c r="F17" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="35"/>
+      <c r="G17" s="29"/>
     </row>
     <row r="18" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="40" t="s">
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
     </row>
     <row r="19" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
@@ -1056,7 +1056,7 @@
     </row>
     <row r="23" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
@@ -1064,7 +1064,7 @@
     </row>
     <row r="24" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
@@ -1092,7 +1092,7 @@
     <row r="42" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="43" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="44" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1116,7 +1116,7 @@
         <v>17</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F54" s="10" t="s">
         <v>18</v>
@@ -1134,24 +1134,24 @@
       <c r="G55" s="23"/>
     </row>
     <row r="56" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="37" t="s">
+      <c r="A56" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B56" s="37"/>
-      <c r="C56" s="37"/>
-      <c r="D56" s="37"/>
-      <c r="E56" s="37"/>
-      <c r="F56" s="37"/>
-      <c r="G56" s="37"/>
-      <c r="H56" s="37"/>
-      <c r="I56" s="37"/>
-      <c r="J56" s="37"/>
-      <c r="K56" s="37"/>
+      <c r="B56" s="31"/>
+      <c r="C56" s="31"/>
+      <c r="D56" s="31"/>
+      <c r="E56" s="31"/>
+      <c r="F56" s="31"/>
+      <c r="G56" s="31"/>
+      <c r="H56" s="31"/>
+      <c r="I56" s="31"/>
+      <c r="J56" s="31"/>
+      <c r="K56" s="31"/>
     </row>
     <row r="57" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1164,25 +1164,25 @@
     <row r="66" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="67" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B67" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C67" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C67" s="10" t="s">
+      <c r="D67" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D67" s="10" t="s">
+      <c r="E67" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E67" s="10" t="s">
+      <c r="F67" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F67" s="10" t="s">
+      <c r="G67" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H67" s="10" t="s">
         <v>39</v>
-      </c>
-      <c r="G67" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="H67" s="10" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="68" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -1197,7 +1197,7 @@
     <row r="69" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="70" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="71" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1210,25 +1210,25 @@
     <row r="78" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="79" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B79" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C79" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C79" s="10" t="s">
+      <c r="D79" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D79" s="10" t="s">
+      <c r="E79" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E79" s="10" t="s">
+      <c r="F79" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F79" s="10" t="s">
+      <c r="G79" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H79" s="10" t="s">
         <v>39</v>
-      </c>
-      <c r="G79" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="H79" s="10" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="80" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -1243,7 +1243,7 @@
     <row r="81" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="82" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="83" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1256,25 +1256,25 @@
     <row r="90" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="91" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B91" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C91" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C91" s="10" t="s">
+      <c r="D91" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D91" s="10" t="s">
+      <c r="E91" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E91" s="10" t="s">
+      <c r="F91" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F91" s="10" t="s">
+      <c r="G91" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H91" s="10" t="s">
         <v>39</v>
-      </c>
-      <c r="G91" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="H91" s="10" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="92" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -1289,7 +1289,7 @@
     <row r="93" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="94" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B94" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="95" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1302,13 +1302,13 @@
     <row r="102" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="103" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B103" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C103" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C103" s="18" t="s">
-        <v>43</v>
-      </c>
       <c r="D103" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E103" s="18" t="s">
         <v>15</v>
@@ -1316,7 +1316,7 @@
       <c r="F103" s="18"/>
       <c r="G103" s="18"/>
       <c r="H103" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="104" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -1331,7 +1331,7 @@
     <row r="105" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="106" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B106" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="107" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1344,19 +1344,19 @@
     <row r="114" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="115" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B115" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C115" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D115" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E115" s="10"/>
       <c r="F115" s="10"/>
       <c r="G115" s="10"/>
       <c r="H115" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="116" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -1371,7 +1371,7 @@
     <row r="117" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="118" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B118" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="119" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1384,21 +1384,21 @@
     <row r="126" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="127" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B127" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C127" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D127" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E127" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F127" s="18"/>
       <c r="G127" s="18"/>
       <c r="H127" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="128" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -1413,7 +1413,7 @@
     <row r="129" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="130" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B130" s="27"/>
       <c r="C130" s="27"/>
@@ -1429,6 +1429,17 @@
     <row r="131" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="E16:G16"/>
     <mergeCell ref="B16:D16"/>
@@ -1444,17 +1455,6 @@
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="A14:K14"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="7.874015748031496E-2" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.19685039370078741"/>

</xml_diff>

<commit_message>
feat: v1.1.0 tech data sheet change
</commit_message>
<xml_diff>
--- a/template/data-worksheet.xlsx
+++ b/template/data-worksheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E9F444-21C6-4BD6-93D9-F5D4F0DA42D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0730F136-2DF0-434C-BBBC-A23A659EF604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="50">
   <si>
-    <t>Версия программы: 1.0.0</t>
-  </si>
-  <si>
     <t>Дата подбора:</t>
   </si>
   <si>
@@ -174,6 +171,9 @@
   </si>
   <si>
     <t>Уровень звуковой мощности, дБ(А):</t>
+  </si>
+  <si>
+    <t>Версия программы: 1.1.0</t>
   </si>
 </sst>
 </file>
@@ -225,9 +225,10 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -236,25 +237,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79992065187536243"/>
+        <fgColor theme="2" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDEEBF7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79995117038483843"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.249977111117893"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -271,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -296,9 +285,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -316,17 +302,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -335,14 +321,29 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -353,35 +354,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -389,6 +372,15 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF5BFFA9"/>
+      <color rgb="FF9BFFEC"/>
+      <color rgb="FF00D0A8"/>
+      <color rgb="FF009779"/>
+      <color rgb="FF27BD99"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -449,15 +441,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>170794</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>105367</xdr:rowOff>
+      <xdr:colOff>129541</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>124810</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>74105</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>510540</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>8033</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -475,19 +467,21 @@
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
             <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
               <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:srcRect/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="170794" y="501607"/>
-          <a:ext cx="1782816" cy="563098"/>
+          <a:off x="129541" y="335280"/>
+          <a:ext cx="2819399" cy="861473"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -808,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K131"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A6" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -818,52 +812,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="40"/>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
+      <c r="A1" s="26"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
     </row>
     <row r="2" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
+      <c r="A2" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
     </row>
     <row r="3" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="5"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
       <c r="G3" s="8"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
     </row>
     <row r="4" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="11"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="H4" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4" s="34"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
+      <c r="C4" s="10"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="H4" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="27"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
     </row>
     <row r="5" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
       <c r="H5" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5" s="3"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
     </row>
     <row r="6" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
@@ -879,19 +873,19 @@
       <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
+      <c r="A7" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
     </row>
     <row r="8" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="9"/>
@@ -906,172 +900,172 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14" t="s">
-        <v>28</v>
+      <c r="B9" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13" t="s">
+        <v>27</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="15"/>
+      <c r="K9" s="14"/>
     </row>
     <row r="10" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14" t="s">
-        <v>29</v>
+      <c r="B10" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13" t="s">
+        <v>28</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="15"/>
+      <c r="K10" s="14"/>
     </row>
     <row r="11" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14" t="s">
-        <v>30</v>
+      <c r="B11" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13" t="s">
+        <v>29</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-      <c r="K11" s="15"/>
+      <c r="K11" s="14"/>
     </row>
     <row r="12" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14" t="s">
-        <v>32</v>
+      <c r="B12" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="I12" s="2"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="15"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="14"/>
     </row>
     <row r="13" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31"/>
+      <c r="A14" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="35"/>
     </row>
     <row r="15" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+    </row>
+    <row r="17" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-    </row>
-    <row r="17" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="29" t="s">
+      <c r="G17" s="33"/>
+    </row>
+    <row r="18" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="29"/>
-    </row>
-    <row r="18" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="30" t="s">
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
     </row>
     <row r="19" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
+        <v>19</v>
+      </c>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
     </row>
     <row r="20" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
+        <v>10</v>
+      </c>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
     </row>
     <row r="21" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
+        <v>11</v>
+      </c>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
     </row>
     <row r="22" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
+        <v>12</v>
+      </c>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
     </row>
     <row r="23" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
+        <v>48</v>
+      </c>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
     </row>
     <row r="24" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="25"/>
+        <v>30</v>
+      </c>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="16"/>
+      <c r="B25" s="15"/>
     </row>
     <row r="26" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1092,7 +1086,7 @@
     <row r="42" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="43" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1106,52 +1100,52 @@
     <row r="52" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="53" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="54" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="10" t="s">
+      <c r="B54" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C54" s="10" t="s">
+      <c r="D54" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D54" s="10" t="s">
+      <c r="E54" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F54" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="E54" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F54" s="10" t="s">
+      <c r="G54" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G54" s="10" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="55" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="23"/>
-      <c r="C55" s="23"/>
-      <c r="D55" s="23"/>
-      <c r="E55" s="23"/>
-      <c r="F55" s="24"/>
-      <c r="G55" s="23"/>
+      <c r="B55" s="22"/>
+      <c r="C55" s="22"/>
+      <c r="D55" s="22"/>
+      <c r="E55" s="22"/>
+      <c r="F55" s="23"/>
+      <c r="G55" s="22"/>
     </row>
     <row r="56" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="B56" s="31"/>
-      <c r="C56" s="31"/>
-      <c r="D56" s="31"/>
-      <c r="E56" s="31"/>
-      <c r="F56" s="31"/>
-      <c r="G56" s="31"/>
-      <c r="H56" s="31"/>
-      <c r="I56" s="31"/>
-      <c r="J56" s="31"/>
-      <c r="K56" s="31"/>
+      <c r="A56" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B56" s="35"/>
+      <c r="C56" s="35"/>
+      <c r="D56" s="35"/>
+      <c r="E56" s="35"/>
+      <c r="F56" s="35"/>
+      <c r="G56" s="35"/>
+      <c r="H56" s="35"/>
+      <c r="I56" s="35"/>
+      <c r="J56" s="35"/>
+      <c r="K56" s="35"/>
     </row>
     <row r="57" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1163,41 +1157,41 @@
     <row r="65" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="66" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="67" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="10" t="s">
+      <c r="B67" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C67" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C67" s="10" t="s">
+      <c r="D67" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="D67" s="10" t="s">
+      <c r="E67" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="E67" s="10" t="s">
+      <c r="F67" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="F67" s="10" t="s">
+      <c r="G67" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="H67" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="G67" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H67" s="10" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="68" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="21"/>
-      <c r="C68" s="21"/>
-      <c r="D68" s="22"/>
-      <c r="E68" s="21"/>
-      <c r="F68" s="21"/>
-      <c r="G68" s="21"/>
-      <c r="H68" s="21"/>
+      <c r="B68" s="24"/>
+      <c r="C68" s="24"/>
+      <c r="D68" s="25"/>
+      <c r="E68" s="24"/>
+      <c r="F68" s="24"/>
+      <c r="G68" s="24"/>
+      <c r="H68" s="24"/>
     </row>
     <row r="69" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="70" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="71" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1209,41 +1203,41 @@
     <row r="77" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="78" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="79" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="10" t="s">
+      <c r="B79" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C79" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C79" s="10" t="s">
+      <c r="D79" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="D79" s="10" t="s">
+      <c r="E79" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="E79" s="10" t="s">
+      <c r="F79" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="F79" s="10" t="s">
+      <c r="G79" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="H79" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="G79" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H79" s="10" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="80" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="21"/>
-      <c r="C80" s="21"/>
-      <c r="D80" s="22"/>
-      <c r="E80" s="21"/>
-      <c r="F80" s="21"/>
-      <c r="G80" s="21"/>
-      <c r="H80" s="21"/>
+      <c r="B80" s="24"/>
+      <c r="C80" s="24"/>
+      <c r="D80" s="25"/>
+      <c r="E80" s="24"/>
+      <c r="F80" s="24"/>
+      <c r="G80" s="24"/>
+      <c r="H80" s="24"/>
     </row>
     <row r="81" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="82" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="83" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1255,45 +1249,45 @@
     <row r="89" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="90" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="91" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="10" t="s">
+      <c r="B91" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C91" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C91" s="10" t="s">
+      <c r="D91" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="D91" s="10" t="s">
+      <c r="E91" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="E91" s="10" t="s">
+      <c r="F91" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="F91" s="10" t="s">
+      <c r="G91" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="H91" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="G91" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H91" s="10" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="92" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="21"/>
-      <c r="C92" s="21"/>
-      <c r="D92" s="22"/>
-      <c r="E92" s="21"/>
-      <c r="F92" s="21"/>
-      <c r="G92" s="21"/>
-      <c r="H92" s="21"/>
+      <c r="B92" s="24"/>
+      <c r="C92" s="24"/>
+      <c r="D92" s="25"/>
+      <c r="E92" s="24"/>
+      <c r="F92" s="24"/>
+      <c r="G92" s="24"/>
+      <c r="H92" s="24"/>
     </row>
     <row r="93" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="94" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B94" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="95" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="96" spans="2:8" s="19" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="96" spans="2:8" s="17" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="97" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="98" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="99" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1301,145 +1295,134 @@
     <row r="101" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="102" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="103" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B103" s="18" t="s">
+      <c r="B103" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C103" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C103" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="D103" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="E103" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="F103" s="18"/>
-      <c r="G103" s="18"/>
-      <c r="H103" s="18" t="s">
+      <c r="D103" s="21" t="s">
         <v>39</v>
       </c>
+      <c r="E103" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F103" s="21"/>
+      <c r="G103" s="21"/>
+      <c r="H103" s="21" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="104" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B104" s="20"/>
-      <c r="C104" s="20"/>
-      <c r="D104" s="20"/>
-      <c r="E104" s="20"/>
-      <c r="F104" s="20"/>
-      <c r="G104" s="20"/>
-      <c r="H104" s="20"/>
+      <c r="B104" s="24"/>
+      <c r="C104" s="24"/>
+      <c r="D104" s="24"/>
+      <c r="E104" s="24"/>
+      <c r="F104" s="24"/>
+      <c r="G104" s="24"/>
+      <c r="H104" s="24"/>
     </row>
     <row r="105" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="106" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B106" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="107" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="108" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="109" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="110" spans="2:8" s="19" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="110" spans="2:8" s="17" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="111" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="112" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="113" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="114" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="115" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B115" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C115" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D115" s="10" t="s">
+      <c r="B115" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C115" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E115" s="10"/>
-      <c r="F115" s="10"/>
-      <c r="G115" s="10"/>
-      <c r="H115" s="10" t="s">
-        <v>39</v>
+      <c r="D115" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="E115" s="21"/>
+      <c r="F115" s="21"/>
+      <c r="G115" s="21"/>
+      <c r="H115" s="21" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="116" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B116" s="21"/>
-      <c r="C116" s="21"/>
-      <c r="D116" s="21"/>
-      <c r="E116" s="21"/>
-      <c r="F116" s="21"/>
-      <c r="G116" s="21"/>
-      <c r="H116" s="21"/>
+      <c r="B116" s="24"/>
+      <c r="C116" s="24"/>
+      <c r="D116" s="24"/>
+      <c r="E116" s="24"/>
+      <c r="F116" s="24"/>
+      <c r="G116" s="24"/>
+      <c r="H116" s="24"/>
     </row>
     <row r="117" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="118" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B118" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="119" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="120" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="121" spans="2:8" s="19" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="121" spans="2:8" s="17" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="122" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="123" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="124" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="125" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="126" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="127" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B127" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C127" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D127" s="18" t="s">
+      <c r="B127" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C127" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E127" s="18" t="s">
+      <c r="D127" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F127" s="18"/>
-      <c r="G127" s="18"/>
-      <c r="H127" s="18" t="s">
-        <v>39</v>
+      <c r="E127" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F127" s="21"/>
+      <c r="G127" s="21"/>
+      <c r="H127" s="21" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="128" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B128" s="20"/>
-      <c r="C128" s="20"/>
-      <c r="D128" s="20"/>
-      <c r="E128" s="20"/>
-      <c r="F128" s="20"/>
-      <c r="G128" s="20"/>
-      <c r="H128" s="20"/>
-    </row>
-    <row r="129" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.3"/>
+      <c r="B128" s="24"/>
+      <c r="C128" s="24"/>
+      <c r="D128" s="24"/>
+      <c r="E128" s="24"/>
+      <c r="F128" s="24"/>
+      <c r="G128" s="24"/>
+      <c r="H128" s="24"/>
+    </row>
+    <row r="129" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="130" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="B130" s="27"/>
-      <c r="C130" s="27"/>
-      <c r="D130" s="27"/>
-      <c r="E130" s="27"/>
-      <c r="F130" s="27"/>
-      <c r="G130" s="27"/>
-      <c r="H130" s="27"/>
-      <c r="I130" s="27"/>
-      <c r="J130" s="27"/>
-      <c r="K130" s="27"/>
+      <c r="A130" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B130" s="20"/>
+      <c r="C130" s="20"/>
+      <c r="D130" s="20"/>
+      <c r="E130" s="20"/>
+      <c r="F130" s="20"/>
+      <c r="G130" s="20"/>
+      <c r="H130" s="20"/>
+      <c r="I130" s="20"/>
+      <c r="J130" s="20"/>
+      <c r="K130" s="20"/>
     </row>
     <row r="131" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="E16:G16"/>
     <mergeCell ref="B16:D16"/>
@@ -1455,6 +1438,17 @@
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="A14:K14"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="7.874015748031496E-2" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.19685039370078741"/>

</xml_diff>

<commit_message>
feat: add fan working point in data sheet
</commit_message>
<xml_diff>
--- a/template/data-worksheet.xlsx
+++ b/template/data-worksheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0730F136-2DF0-434C-BBBC-A23A659EF604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55FA3DDD-A005-45C6-AD05-518529F2D47F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Техника" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
   <si>
     <t>Дата подбора:</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>Версия программы: 1.1.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фактическая рабочая точка: </t>
   </si>
 </sst>
 </file>
@@ -260,7 +263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -327,6 +330,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -350,9 +357,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -802,49 +806,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K131"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:F4"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A14" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25:G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26"/>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-    </row>
-    <row r="2" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
+    <row r="1" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A1" s="28"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+    </row>
+    <row r="2" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A2" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-    </row>
-    <row r="3" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+    </row>
+    <row r="3" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="1">
       <c r="A3" s="5"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
       <c r="G3" s="8"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-    </row>
-    <row r="4" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+    </row>
+    <row r="4" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="C4" s="10"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="H4" s="27" t="s">
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="H4" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="27"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-    </row>
-    <row r="5" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I4" s="29"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+    </row>
+    <row r="5" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="12"/>
@@ -856,10 +860,10 @@
         <v>0</v>
       </c>
       <c r="I5" s="3"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-    </row>
-    <row r="6" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+    </row>
+    <row r="6" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="7"/>
@@ -872,22 +876,22 @@
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="36" t="s">
+    <row r="7" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A7" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="36"/>
-    </row>
-    <row r="8" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+    </row>
+    <row r="8" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -899,14 +903,14 @@
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
     </row>
-    <row r="9" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="27" t="s">
+    <row r="9" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B9" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
       <c r="G9" s="13"/>
       <c r="H9" s="13" t="s">
         <v>27</v>
@@ -915,14 +919,14 @@
       <c r="J9" s="2"/>
       <c r="K9" s="14"/>
     </row>
-    <row r="10" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="27" t="s">
+    <row r="10" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B10" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
       <c r="G10" s="13"/>
       <c r="H10" s="13" t="s">
         <v>28</v>
@@ -931,14 +935,14 @@
       <c r="J10" s="2"/>
       <c r="K10" s="14"/>
     </row>
-    <row r="11" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="27" t="s">
+    <row r="11" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B11" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13" t="s">
         <v>29</v>
@@ -947,14 +951,14 @@
       <c r="J11" s="2"/>
       <c r="K11" s="14"/>
     </row>
-    <row r="12" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="27" t="s">
+    <row r="12" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B12" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
       <c r="G12" s="13"/>
       <c r="H12" s="13" t="s">
         <v>31</v>
@@ -963,68 +967,68 @@
       <c r="J12" s="19"/>
       <c r="K12" s="14"/>
     </row>
-    <row r="13" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="35" t="s">
+    <row r="13" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="14" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A14" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="35"/>
-    </row>
-    <row r="15" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="34" t="s">
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="36"/>
+    </row>
+    <row r="15" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="16" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B16" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="33" t="s">
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-    </row>
-    <row r="17" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="34" t="s">
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+    </row>
+    <row r="17" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B17" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="33" t="s">
+      <c r="F17" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="G17" s="33"/>
-    </row>
-    <row r="18" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="34" t="s">
+      <c r="G17" s="35"/>
+    </row>
+    <row r="18" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B18" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="38" t="s">
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-    </row>
-    <row r="19" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="3" t="s">
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+    </row>
+    <row r="19" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B19" s="26" t="s">
         <v>19</v>
       </c>
       <c r="E19" s="16"/>
       <c r="F19" s="16"/>
       <c r="G19" s="16"/>
     </row>
-    <row r="20" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B20" s="3" t="s">
         <v>10</v>
       </c>
@@ -1032,7 +1036,7 @@
       <c r="F20" s="16"/>
       <c r="G20" s="16"/>
     </row>
-    <row r="21" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B21" s="3" t="s">
         <v>11</v>
       </c>
@@ -1040,7 +1044,7 @@
       <c r="F21" s="16"/>
       <c r="G21" s="16"/>
     </row>
-    <row r="22" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B22" s="3" t="s">
         <v>12</v>
       </c>
@@ -1048,7 +1052,7 @@
       <c r="F22" s="16"/>
       <c r="G22" s="16"/>
     </row>
-    <row r="23" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B23" s="3" t="s">
         <v>48</v>
       </c>
@@ -1056,7 +1060,7 @@
       <c r="F23" s="16"/>
       <c r="G23" s="16"/>
     </row>
-    <row r="24" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B24" s="3" t="s">
         <v>30</v>
       </c>
@@ -1064,42 +1068,47 @@
       <c r="F24" s="16"/>
       <c r="G24" s="18"/>
     </row>
-    <row r="25" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="15"/>
-    </row>
-    <row r="26" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="34" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="35" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="36" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B25" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25" s="35"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="35"/>
+    </row>
+    <row r="26" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="27" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="28" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="29" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="30" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="31" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="32" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="33" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="34" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="35" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="36" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="37" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="38" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="39" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="40" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="41" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="42" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="43" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B43" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="2:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="49" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="50" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="51" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="52" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="53" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="54" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="45" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="46" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="47" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="48" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="49" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="50" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="51" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="52" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="53" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="54" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B54" s="21" t="s">
         <v>14</v>
       </c>
@@ -1119,7 +1128,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B55" s="22"/>
       <c r="C55" s="22"/>
       <c r="D55" s="22"/>
@@ -1127,36 +1136,36 @@
       <c r="F55" s="23"/>
       <c r="G55" s="22"/>
     </row>
-    <row r="56" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="35" t="s">
+    <row r="56" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A56" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B56" s="35"/>
-      <c r="C56" s="35"/>
-      <c r="D56" s="35"/>
-      <c r="E56" s="35"/>
-      <c r="F56" s="35"/>
-      <c r="G56" s="35"/>
-      <c r="H56" s="35"/>
-      <c r="I56" s="35"/>
-      <c r="J56" s="35"/>
-      <c r="K56" s="35"/>
-    </row>
-    <row r="57" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="58" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="36"/>
+      <c r="C56" s="36"/>
+      <c r="D56" s="36"/>
+      <c r="E56" s="36"/>
+      <c r="F56" s="36"/>
+      <c r="G56" s="36"/>
+      <c r="H56" s="36"/>
+      <c r="I56" s="36"/>
+      <c r="J56" s="36"/>
+      <c r="K56" s="36"/>
+    </row>
+    <row r="57" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="58" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B58" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="60" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="61" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="62" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="63" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="64" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="65" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="66" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="67" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="60" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="61" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="62" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="63" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="64" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="65" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="66" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="67" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B67" s="21" t="s">
         <v>33</v>
       </c>
@@ -1179,7 +1188,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="68" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B68" s="24"/>
       <c r="C68" s="24"/>
       <c r="D68" s="25"/>
@@ -1188,21 +1197,21 @@
       <c r="G68" s="24"/>
       <c r="H68" s="24"/>
     </row>
-    <row r="69" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="70" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="70" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B70" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="71" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="72" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="73" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="74" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="75" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="76" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="77" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="78" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="79" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="72" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="73" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="74" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="75" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="76" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="77" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="78" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="79" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B79" s="21" t="s">
         <v>33</v>
       </c>
@@ -1225,7 +1234,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="80" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B80" s="24"/>
       <c r="C80" s="24"/>
       <c r="D80" s="25"/>
@@ -1234,21 +1243,21 @@
       <c r="G80" s="24"/>
       <c r="H80" s="24"/>
     </row>
-    <row r="81" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="82" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="82" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B82" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="83" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="84" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="85" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="86" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="87" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="88" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="89" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="90" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="91" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="84" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="85" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="86" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="87" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="88" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="89" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="90" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="91" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B91" s="21" t="s">
         <v>33</v>
       </c>
@@ -1271,7 +1280,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="92" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B92" s="24"/>
       <c r="C92" s="24"/>
       <c r="D92" s="25"/>
@@ -1280,21 +1289,21 @@
       <c r="G92" s="24"/>
       <c r="H92" s="24"/>
     </row>
-    <row r="93" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="94" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="94" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B94" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="95" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="96" spans="2:8" s="17" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="97" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="98" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="99" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="100" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="101" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="102" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="103" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="96" spans="2:8" s="17" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="97" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="98" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="99" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="100" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="101" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="102" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="103" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B103" s="21" t="s">
         <v>40</v>
       </c>
@@ -1313,7 +1322,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="104" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B104" s="24"/>
       <c r="C104" s="24"/>
       <c r="D104" s="24"/>
@@ -1322,21 +1331,21 @@
       <c r="G104" s="24"/>
       <c r="H104" s="24"/>
     </row>
-    <row r="105" spans="2:8" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="106" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="106" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B106" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="107" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="108" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="109" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="110" spans="2:8" s="17" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="111" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="112" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="113" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="114" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="115" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="108" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="109" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="110" spans="2:8" s="17" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="111" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="112" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="113" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="114" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="115" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B115" s="21" t="s">
         <v>39</v>
       </c>
@@ -1353,7 +1362,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="116" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B116" s="24"/>
       <c r="C116" s="24"/>
       <c r="D116" s="24"/>
@@ -1362,21 +1371,21 @@
       <c r="G116" s="24"/>
       <c r="H116" s="24"/>
     </row>
-    <row r="117" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="118" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="118" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B118" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="119" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="120" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="121" spans="2:8" s="17" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="122" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="123" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="124" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="125" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="126" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="127" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="120" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="121" spans="2:8" s="17" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="122" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="123" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="124" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="125" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="126" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="127" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B127" s="21" t="s">
         <v>42</v>
       </c>
@@ -1395,7 +1404,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="128" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B128" s="24"/>
       <c r="C128" s="24"/>
       <c r="D128" s="24"/>
@@ -1404,8 +1413,8 @@
       <c r="G128" s="24"/>
       <c r="H128" s="24"/>
     </row>
-    <row r="129" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="130" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.75"/>
+    <row r="130" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A130" s="20" t="s">
         <v>46</v>
       </c>
@@ -1420,12 +1429,11 @@
       <c r="J130" s="20"/>
       <c r="K130" s="20"/>
     </row>
-    <row r="131" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="131" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="24">
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="E16:G16"/>
-    <mergeCell ref="B16:D16"/>
     <mergeCell ref="A56:K56"/>
     <mergeCell ref="A7:K7"/>
     <mergeCell ref="E12:F12"/>
@@ -1433,11 +1441,10 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="A14:K14"/>
+    <mergeCell ref="E25:G25"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="E3:F3"/>

</xml_diff>

<commit_message>
feat: add new version name in datasheet
</commit_message>
<xml_diff>
--- a/template/data-worksheet.xlsx
+++ b/template/data-worksheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55FA3DDD-A005-45C6-AD05-518529F2D47F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7176C3-84D8-465C-84CB-28DDAED7734D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -173,10 +173,10 @@
     <t>Уровень звуковой мощности, дБ(А):</t>
   </si>
   <si>
-    <t>Версия программы: 1.1.0</t>
-  </si>
-  <si>
     <t xml:space="preserve">Фактическая рабочая точка: </t>
+  </si>
+  <si>
+    <t>Версия программы: 1.2.0</t>
   </si>
 </sst>
 </file>
@@ -334,41 +334,41 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -806,8 +806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K131"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A14" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25:G25"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -816,37 +816,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="28"/>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
+      <c r="A1" s="39"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
     </row>
     <row r="2" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A2" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
+      <c r="A2" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
     </row>
     <row r="3" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="1">
       <c r="A3" s="5"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
       <c r="G3" s="8"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
     </row>
     <row r="4" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="C4" s="10"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="H4" s="29" t="s">
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="H4" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="29"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="31"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
     </row>
     <row r="5" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A5" s="11"/>
@@ -860,8 +860,8 @@
         <v>0</v>
       </c>
       <c r="I5" s="3"/>
-      <c r="J5" s="34"/>
-      <c r="K5" s="34"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
     </row>
     <row r="6" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A6" s="6"/>
@@ -877,19 +877,19 @@
       <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
     </row>
     <row r="8" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B8" s="9"/>
@@ -904,13 +904,13 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
       <c r="G9" s="13"/>
       <c r="H9" s="13" t="s">
         <v>27</v>
@@ -920,13 +920,13 @@
       <c r="K9" s="14"/>
     </row>
     <row r="10" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
       <c r="G10" s="13"/>
       <c r="H10" s="13" t="s">
         <v>28</v>
@@ -936,13 +936,13 @@
       <c r="K10" s="14"/>
     </row>
     <row r="11" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13" t="s">
         <v>29</v>
@@ -952,13 +952,13 @@
       <c r="K11" s="14"/>
     </row>
     <row r="12" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
       <c r="G12" s="13"/>
       <c r="H12" s="13" t="s">
         <v>31</v>
@@ -969,19 +969,19 @@
     </row>
     <row r="13" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
     <row r="14" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="36"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="36"/>
-      <c r="K14" s="36"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
     </row>
     <row r="15" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
     <row r="16" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
@@ -990,11 +990,11 @@
       </c>
       <c r="C16" s="27"/>
       <c r="D16" s="27"/>
-      <c r="E16" s="35" t="s">
+      <c r="E16" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
     </row>
     <row r="17" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B17" s="27" t="s">
@@ -1003,10 +1003,10 @@
       <c r="C17" s="27"/>
       <c r="D17" s="27"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="35" t="s">
+      <c r="F17" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G17" s="35"/>
+      <c r="G17" s="29"/>
     </row>
     <row r="18" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B18" s="27" t="s">
@@ -1014,11 +1014,11 @@
       </c>
       <c r="C18" s="27"/>
       <c r="D18" s="27"/>
-      <c r="E18" s="39" t="s">
+      <c r="E18" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
     </row>
     <row r="19" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B19" s="26" t="s">
@@ -1070,11 +1070,11 @@
     </row>
     <row r="25" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B25" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="35"/>
+        <v>49</v>
+      </c>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
     </row>
     <row r="26" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
     <row r="27" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
@@ -1137,19 +1137,19 @@
       <c r="G55" s="22"/>
     </row>
     <row r="56" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A56" s="36" t="s">
+      <c r="A56" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B56" s="36"/>
-      <c r="C56" s="36"/>
-      <c r="D56" s="36"/>
-      <c r="E56" s="36"/>
-      <c r="F56" s="36"/>
-      <c r="G56" s="36"/>
-      <c r="H56" s="36"/>
-      <c r="I56" s="36"/>
-      <c r="J56" s="36"/>
-      <c r="K56" s="36"/>
+      <c r="B56" s="30"/>
+      <c r="C56" s="30"/>
+      <c r="D56" s="30"/>
+      <c r="E56" s="30"/>
+      <c r="F56" s="30"/>
+      <c r="G56" s="30"/>
+      <c r="H56" s="30"/>
+      <c r="I56" s="30"/>
+      <c r="J56" s="30"/>
+      <c r="K56" s="30"/>
     </row>
     <row r="57" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
     <row r="58" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
@@ -1432,6 +1432,17 @@
     <row r="131" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="E16:G16"/>
     <mergeCell ref="A56:K56"/>
@@ -1445,17 +1456,6 @@
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="A14:K14"/>
     <mergeCell ref="E25:G25"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="7.874015748031496E-2" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.19685039370078741"/>

</xml_diff>

<commit_message>
feat: update datasheet template
</commit_message>
<xml_diff>
--- a/template/data-worksheet.xlsx
+++ b/template/data-worksheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7176C3-84D8-465C-84CB-28DDAED7734D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8508DC-6597-43B2-BC92-1CA72A1C6D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,12 +50,6 @@
     <t>У1</t>
   </si>
   <si>
-    <t>Температурный диапазон:</t>
-  </si>
-  <si>
-    <t>-40 ... +60 ˚С</t>
-  </si>
-  <si>
     <t>Электропотребление, кВт:</t>
   </si>
   <si>
@@ -98,9 +92,6 @@
     <t>Габариты:</t>
   </si>
   <si>
-    <t>Расход воздуха, м3/ч:</t>
-  </si>
-  <si>
     <t>Потери сети, Па:</t>
   </si>
   <si>
@@ -173,10 +164,19 @@
     <t>Уровень звуковой мощности, дБ(А):</t>
   </si>
   <si>
-    <t xml:space="preserve">Фактическая рабочая точка: </t>
-  </si>
-  <si>
     <t>Версия программы: 1.2.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фактическая рабочая точка, м³/час / Па: </t>
+  </si>
+  <si>
+    <t>Расход воздуха, м³/ч:</t>
+  </si>
+  <si>
+    <t>-40 ... +60</t>
+  </si>
+  <si>
+    <t>Температурный диапазон, ˚С:</t>
   </si>
 </sst>
 </file>
@@ -263,7 +263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -334,6 +334,27 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -349,26 +370,8 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -806,8 +809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K131"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -816,37 +819,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="39"/>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
+      <c r="A1" s="29"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A2" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
+      <c r="A2" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
     </row>
     <row r="3" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="1">
       <c r="A3" s="5"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
       <c r="G3" s="8"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
     </row>
     <row r="4" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="C4" s="10"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="H4" s="33" t="s">
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="H4" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="33"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
     </row>
     <row r="5" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A5" s="11"/>
@@ -860,8 +863,8 @@
         <v>0</v>
       </c>
       <c r="I5" s="3"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
     </row>
     <row r="6" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A6" s="6"/>
@@ -877,19 +880,19 @@
       <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
     </row>
     <row r="8" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B8" s="9"/>
@@ -904,64 +907,64 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B9" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
+      <c r="B9" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="13"/>
       <c r="H9" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="14"/>
     </row>
     <row r="10" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B10" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
+      <c r="B10" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="13"/>
       <c r="H10" s="13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="14"/>
     </row>
     <row r="11" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B11" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
+      <c r="B11" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="14"/>
     </row>
     <row r="12" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B12" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
+      <c r="B12" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
       <c r="G12" s="13"/>
       <c r="H12" s="13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="19"/>
@@ -969,19 +972,19 @@
     </row>
     <row r="13" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
     <row r="14" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="37"/>
     </row>
     <row r="15" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
     <row r="16" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
@@ -990,11 +993,11 @@
       </c>
       <c r="C16" s="27"/>
       <c r="D16" s="27"/>
-      <c r="E16" s="29" t="s">
+      <c r="E16" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
     </row>
     <row r="17" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B17" s="27" t="s">
@@ -1003,26 +1006,26 @@
       <c r="C17" s="27"/>
       <c r="D17" s="27"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="29" t="s">
+      <c r="F17" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="G17" s="29"/>
+      <c r="G17" s="36"/>
     </row>
     <row r="18" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B18" s="27" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="C18" s="27"/>
       <c r="D18" s="27"/>
-      <c r="E18" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
+      <c r="E18" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
     </row>
     <row r="19" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B19" s="26" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E19" s="16"/>
       <c r="F19" s="16"/>
@@ -1030,7 +1033,7 @@
     </row>
     <row r="20" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B20" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E20" s="16"/>
       <c r="F20" s="16"/>
@@ -1038,7 +1041,7 @@
     </row>
     <row r="21" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B21" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E21" s="16"/>
       <c r="F21" s="16"/>
@@ -1046,7 +1049,7 @@
     </row>
     <row r="22" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B22" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E22" s="16"/>
       <c r="F22" s="16"/>
@@ -1054,7 +1057,7 @@
     </row>
     <row r="23" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B23" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E23" s="16"/>
       <c r="F23" s="16"/>
@@ -1062,7 +1065,7 @@
     </row>
     <row r="24" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B24" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E24" s="16"/>
       <c r="F24" s="16"/>
@@ -1070,11 +1073,11 @@
     </row>
     <row r="25" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B25" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
+        <v>47</v>
+      </c>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="28"/>
     </row>
     <row r="26" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
     <row r="27" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
@@ -1095,7 +1098,7 @@
     <row r="42" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
     <row r="43" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B43" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="44" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
@@ -1110,22 +1113,22 @@
     <row r="53" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
     <row r="54" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B54" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C54" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C54" s="21" t="s">
+      <c r="E54" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F54" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D54" s="21" t="s">
+      <c r="G54" s="21" t="s">
         <v>16</v>
-      </c>
-      <c r="E54" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="F54" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="G54" s="21" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
@@ -1137,24 +1140,24 @@
       <c r="G55" s="22"/>
     </row>
     <row r="56" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A56" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="B56" s="30"/>
-      <c r="C56" s="30"/>
-      <c r="D56" s="30"/>
-      <c r="E56" s="30"/>
-      <c r="F56" s="30"/>
-      <c r="G56" s="30"/>
-      <c r="H56" s="30"/>
-      <c r="I56" s="30"/>
-      <c r="J56" s="30"/>
-      <c r="K56" s="30"/>
+      <c r="A56" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="B56" s="37"/>
+      <c r="C56" s="37"/>
+      <c r="D56" s="37"/>
+      <c r="E56" s="37"/>
+      <c r="F56" s="37"/>
+      <c r="G56" s="37"/>
+      <c r="H56" s="37"/>
+      <c r="I56" s="37"/>
+      <c r="J56" s="37"/>
+      <c r="K56" s="37"/>
     </row>
     <row r="57" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
     <row r="58" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B58" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
@@ -1167,25 +1170,25 @@
     <row r="66" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
     <row r="67" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B67" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C67" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D67" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E67" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C67" s="21" t="s">
+      <c r="F67" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="D67" s="21" t="s">
+      <c r="G67" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="H67" s="21" t="s">
         <v>35</v>
-      </c>
-      <c r="E67" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="F67" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="G67" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="H67" s="21" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="68" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
@@ -1200,7 +1203,7 @@
     <row r="69" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
     <row r="70" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B70" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="71" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
@@ -1213,25 +1216,25 @@
     <row r="78" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
     <row r="79" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B79" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C79" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D79" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E79" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C79" s="21" t="s">
+      <c r="F79" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="D79" s="21" t="s">
+      <c r="G79" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="H79" s="21" t="s">
         <v>35</v>
-      </c>
-      <c r="E79" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="F79" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="G79" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="H79" s="21" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="80" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
@@ -1246,7 +1249,7 @@
     <row r="81" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
     <row r="82" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B82" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="83" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
@@ -1259,25 +1262,25 @@
     <row r="90" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
     <row r="91" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B91" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C91" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D91" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E91" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C91" s="21" t="s">
+      <c r="F91" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="D91" s="21" t="s">
+      <c r="G91" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="H91" s="21" t="s">
         <v>35</v>
-      </c>
-      <c r="E91" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="F91" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="G91" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="H91" s="21" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="92" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
@@ -1292,7 +1295,7 @@
     <row r="93" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
     <row r="94" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B94" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="95" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
@@ -1305,21 +1308,21 @@
     <row r="102" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
     <row r="103" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B103" s="21" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C103" s="21" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D103" s="21" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E103" s="21" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F103" s="21"/>
       <c r="G103" s="21"/>
       <c r="H103" s="21" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="104" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
@@ -1334,7 +1337,7 @@
     <row r="105" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
     <row r="106" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B106" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="107" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
@@ -1347,19 +1350,19 @@
     <row r="114" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
     <row r="115" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B115" s="21" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C115" s="21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D115" s="21" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E115" s="21"/>
       <c r="F115" s="21"/>
       <c r="G115" s="21"/>
       <c r="H115" s="21" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="116" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
@@ -1374,7 +1377,7 @@
     <row r="117" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
     <row r="118" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B118" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="119" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
@@ -1387,21 +1390,21 @@
     <row r="126" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
     <row r="127" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B127" s="21" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C127" s="21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D127" s="21" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E127" s="21" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F127" s="21"/>
       <c r="G127" s="21"/>
       <c r="H127" s="21" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="128" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
@@ -1416,7 +1419,7 @@
     <row r="129" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.75"/>
     <row r="130" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A130" s="20" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B130" s="20"/>
       <c r="C130" s="20"/>
@@ -1431,18 +1434,7 @@
     </row>
     <row r="131" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
+  <mergeCells count="23">
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="E16:G16"/>
     <mergeCell ref="A56:K56"/>
@@ -1455,7 +1447,17 @@
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="A14:K14"/>
-    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="7.874015748031496E-2" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.19685039370078741"/>

</xml_diff>

<commit_message>
hotfix: fix connection reset for db 2
</commit_message>
<xml_diff>
--- a/template/data-worksheet.xlsx
+++ b/template/data-worksheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8508DC-6597-43B2-BC92-1CA72A1C6D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380712CD-8882-4C9E-B739-3DA770FCF116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Техника" sheetId="1" r:id="rId1"/>
@@ -164,9 +164,6 @@
     <t>Уровень звуковой мощности, дБ(А):</t>
   </si>
   <si>
-    <t>Версия программы: 1.2.0</t>
-  </si>
-  <si>
     <t xml:space="preserve">Фактическая рабочая точка, м³/час / Па: </t>
   </si>
   <si>
@@ -177,6 +174,9 @@
   </si>
   <si>
     <t>Температурный диапазон, ˚С:</t>
+  </si>
+  <si>
+    <t>Версия программы: 1.2.1</t>
   </si>
 </sst>
 </file>
@@ -337,41 +337,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -809,49 +809,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K131"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="11" max="11" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="29"/>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-    </row>
-    <row r="2" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A2" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-    </row>
-    <row r="3" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="1">
+    <row r="1" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="40"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+    </row>
+    <row r="2" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+    </row>
+    <row r="3" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
       <c r="G3" s="8"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
-    </row>
-    <row r="4" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+    </row>
+    <row r="4" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="10"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="H4" s="30" t="s">
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="H4" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="30"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
-    </row>
-    <row r="5" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="I4" s="34"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+    </row>
+    <row r="5" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="12"/>
@@ -863,10 +863,10 @@
         <v>0</v>
       </c>
       <c r="I5" s="3"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
-    </row>
-    <row r="6" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+    </row>
+    <row r="6" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="7"/>
@@ -879,22 +879,22 @@
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A7" s="38" t="s">
+    <row r="7" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-    </row>
-    <row r="8" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+    </row>
+    <row r="8" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -906,14 +906,14 @@
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
     </row>
-    <row r="9" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B9" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
+    <row r="9" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
       <c r="G9" s="13"/>
       <c r="H9" s="13" t="s">
         <v>24</v>
@@ -922,14 +922,14 @@
       <c r="J9" s="2"/>
       <c r="K9" s="14"/>
     </row>
-    <row r="10" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B10" s="30" t="s">
+    <row r="10" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
       <c r="G10" s="13"/>
       <c r="H10" s="13" t="s">
         <v>25</v>
@@ -938,14 +938,14 @@
       <c r="J10" s="2"/>
       <c r="K10" s="14"/>
     </row>
-    <row r="11" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B11" s="30" t="s">
+    <row r="11" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13" t="s">
         <v>26</v>
@@ -954,14 +954,14 @@
       <c r="J11" s="2"/>
       <c r="K11" s="14"/>
     </row>
-    <row r="12" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B12" s="30" t="s">
+    <row r="12" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
       <c r="G12" s="13"/>
       <c r="H12" s="13" t="s">
         <v>28</v>
@@ -970,60 +970,60 @@
       <c r="J12" s="19"/>
       <c r="K12" s="14"/>
     </row>
-    <row r="13" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="14" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A14" s="37" t="s">
+    <row r="13" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="37"/>
-    </row>
-    <row r="15" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="16" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
+    </row>
+    <row r="15" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="27" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="27"/>
       <c r="D16" s="27"/>
-      <c r="E16" s="36" t="s">
+      <c r="E16" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-    </row>
-    <row r="17" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+    </row>
+    <row r="17" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="27" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="27"/>
       <c r="D17" s="27"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="36" t="s">
+      <c r="F17" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="G17" s="36"/>
-    </row>
-    <row r="18" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="G17" s="30"/>
+    </row>
+    <row r="18" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18" s="27"/>
       <c r="D18" s="27"/>
-      <c r="E18" s="40" t="s">
-        <v>49</v>
-      </c>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-    </row>
-    <row r="19" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="E18" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+    </row>
+    <row r="19" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="26" t="s">
         <v>17</v>
       </c>
@@ -1031,7 +1031,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="16"/>
     </row>
-    <row r="20" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="20" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>8</v>
       </c>
@@ -1039,7 +1039,7 @@
       <c r="F20" s="16"/>
       <c r="G20" s="16"/>
     </row>
-    <row r="21" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="21" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>9</v>
       </c>
@@ -1047,7 +1047,7 @@
       <c r="F21" s="16"/>
       <c r="G21" s="16"/>
     </row>
-    <row r="22" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="22" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>10</v>
       </c>
@@ -1055,7 +1055,7 @@
       <c r="F22" s="16"/>
       <c r="G22" s="16"/>
     </row>
-    <row r="23" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="23" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>45</v>
       </c>
@@ -1063,7 +1063,7 @@
       <c r="F23" s="16"/>
       <c r="G23" s="16"/>
     </row>
-    <row r="24" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="24" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>27</v>
       </c>
@@ -1071,47 +1071,47 @@
       <c r="F24" s="16"/>
       <c r="G24" s="18"/>
     </row>
-    <row r="25" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="25" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E25" s="27"/>
       <c r="F25" s="27"/>
       <c r="G25" s="28"/>
     </row>
-    <row r="26" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="27" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="28" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="29" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="30" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="31" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="32" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="33" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="34" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="35" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="36" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="37" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="38" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="39" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="40" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="41" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="42" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="43" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="26" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="45" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="46" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="47" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="48" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="49" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="50" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="51" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="52" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="53" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="54" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="44" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="21" t="s">
         <v>12</v>
       </c>
@@ -1131,7 +1131,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="55" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="22"/>
       <c r="C55" s="22"/>
       <c r="D55" s="22"/>
@@ -1139,36 +1139,36 @@
       <c r="F55" s="23"/>
       <c r="G55" s="22"/>
     </row>
-    <row r="56" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A56" s="37" t="s">
+    <row r="56" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B56" s="37"/>
-      <c r="C56" s="37"/>
-      <c r="D56" s="37"/>
-      <c r="E56" s="37"/>
-      <c r="F56" s="37"/>
-      <c r="G56" s="37"/>
-      <c r="H56" s="37"/>
-      <c r="I56" s="37"/>
-      <c r="J56" s="37"/>
-      <c r="K56" s="37"/>
-    </row>
-    <row r="57" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="58" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B56" s="31"/>
+      <c r="C56" s="31"/>
+      <c r="D56" s="31"/>
+      <c r="E56" s="31"/>
+      <c r="F56" s="31"/>
+      <c r="G56" s="31"/>
+      <c r="H56" s="31"/>
+      <c r="I56" s="31"/>
+      <c r="J56" s="31"/>
+      <c r="K56" s="31"/>
+    </row>
+    <row r="57" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="60" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="61" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="62" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="63" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="64" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="65" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="66" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="67" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="59" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="21" t="s">
         <v>30</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="68" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="68" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="24"/>
       <c r="C68" s="24"/>
       <c r="D68" s="25"/>
@@ -1200,21 +1200,21 @@
       <c r="G68" s="24"/>
       <c r="H68" s="24"/>
     </row>
-    <row r="69" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="70" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="69" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="71" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="72" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="73" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="74" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="75" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="76" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="77" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="78" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="79" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="71" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="21" t="s">
         <v>30</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="80" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="80" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="24"/>
       <c r="C80" s="24"/>
       <c r="D80" s="25"/>
@@ -1246,21 +1246,21 @@
       <c r="G80" s="24"/>
       <c r="H80" s="24"/>
     </row>
-    <row r="81" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="82" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="81" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="83" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="84" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="85" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="86" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="87" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="88" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="89" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="90" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="91" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="83" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="21" t="s">
         <v>30</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="92" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="92" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="24"/>
       <c r="C92" s="24"/>
       <c r="D92" s="25"/>
@@ -1292,21 +1292,21 @@
       <c r="G92" s="24"/>
       <c r="H92" s="24"/>
     </row>
-    <row r="93" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="94" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="93" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="95" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="96" spans="2:8" s="17" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="97" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="98" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="99" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="100" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="101" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="102" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="103" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="95" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" spans="2:8" s="17" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" s="21" t="s">
         <v>37</v>
       </c>
@@ -1325,7 +1325,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="104" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="104" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B104" s="24"/>
       <c r="C104" s="24"/>
       <c r="D104" s="24"/>
@@ -1334,21 +1334,21 @@
       <c r="G104" s="24"/>
       <c r="H104" s="24"/>
     </row>
-    <row r="105" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="106" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="105" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="107" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="108" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="109" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="110" spans="2:8" s="17" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="111" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="112" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="113" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="114" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="115" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="107" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" spans="2:8" s="17" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B115" s="21" t="s">
         <v>36</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="116" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="116" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B116" s="24"/>
       <c r="C116" s="24"/>
       <c r="D116" s="24"/>
@@ -1374,21 +1374,21 @@
       <c r="G116" s="24"/>
       <c r="H116" s="24"/>
     </row>
-    <row r="117" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="118" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="117" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="119" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="120" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="121" spans="2:8" s="17" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="122" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="123" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="124" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="125" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="126" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="127" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="119" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" spans="2:8" s="17" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B127" s="21" t="s">
         <v>39</v>
       </c>
@@ -1407,7 +1407,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="128" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="128" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B128" s="24"/>
       <c r="C128" s="24"/>
       <c r="D128" s="24"/>
@@ -1416,8 +1416,8 @@
       <c r="G128" s="24"/>
       <c r="H128" s="24"/>
     </row>
-    <row r="129" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.75"/>
-    <row r="130" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="129" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="130" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="20" t="s">
         <v>43</v>
       </c>
@@ -1432,9 +1432,20 @@
       <c r="J130" s="20"/>
       <c r="K130" s="20"/>
     </row>
-    <row r="131" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="131" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="E16:G16"/>
     <mergeCell ref="A56:K56"/>
@@ -1447,17 +1458,6 @@
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="A14:K14"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="7.874015748031496E-2" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.19685039370078741"/>

</xml_diff>

<commit_message>
feat: add quantity in commercial offer, v1.3.0
</commit_message>
<xml_diff>
--- a/template/data-worksheet.xlsx
+++ b/template/data-worksheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380712CD-8882-4C9E-B739-3DA770FCF116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E63867-6FBE-4230-B658-6C4FE5270C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Техника" sheetId="1" r:id="rId1"/>
@@ -176,7 +176,7 @@
     <t>Температурный диапазон, ˚С:</t>
   </si>
   <si>
-    <t>Версия программы: 1.2.1</t>
+    <t>Версия программы: 1.3.0</t>
   </si>
 </sst>
 </file>
@@ -337,6 +337,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -352,26 +370,8 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -810,48 +810,48 @@
   <dimension ref="A1:K131"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="40"/>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-    </row>
-    <row r="2" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
+    <row r="1" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="29"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+    </row>
+    <row r="2" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-    </row>
-    <row r="3" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+    </row>
+    <row r="3" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="5"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
       <c r="G3" s="8"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-    </row>
-    <row r="4" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+    </row>
+    <row r="4" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C4" s="10"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="H4" s="34" t="s">
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="H4" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="34"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-    </row>
-    <row r="5" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I4" s="30"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+    </row>
+    <row r="5" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="12"/>
@@ -863,10 +863,10 @@
         <v>0</v>
       </c>
       <c r="I5" s="3"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-    </row>
-    <row r="6" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+    </row>
+    <row r="6" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="7"/>
@@ -879,22 +879,22 @@
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
+    <row r="7" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
-    </row>
-    <row r="8" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+    </row>
+    <row r="8" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -906,14 +906,14 @@
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
     </row>
-    <row r="9" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="34" t="s">
+    <row r="9" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="13"/>
       <c r="H9" s="13" t="s">
         <v>24</v>
@@ -922,14 +922,14 @@
       <c r="J9" s="2"/>
       <c r="K9" s="14"/>
     </row>
-    <row r="10" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="34" t="s">
+    <row r="10" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="13"/>
       <c r="H10" s="13" t="s">
         <v>25</v>
@@ -938,14 +938,14 @@
       <c r="J10" s="2"/>
       <c r="K10" s="14"/>
     </row>
-    <row r="11" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="34" t="s">
+    <row r="11" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13" t="s">
         <v>26</v>
@@ -954,14 +954,14 @@
       <c r="J11" s="2"/>
       <c r="K11" s="14"/>
     </row>
-    <row r="12" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="34" t="s">
+    <row r="12" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
       <c r="G12" s="13"/>
       <c r="H12" s="13" t="s">
         <v>28</v>
@@ -970,60 +970,60 @@
       <c r="J12" s="19"/>
       <c r="K12" s="14"/>
     </row>
-    <row r="13" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
+    <row r="13" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31"/>
-    </row>
-    <row r="15" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="37"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="37"/>
+    </row>
+    <row r="15" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="27" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="27"/>
       <c r="D16" s="27"/>
-      <c r="E16" s="30" t="s">
+      <c r="E16" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-    </row>
-    <row r="17" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+    </row>
+    <row r="17" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="27" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="27"/>
       <c r="D17" s="27"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="30" t="s">
+      <c r="F17" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="G17" s="30"/>
-    </row>
-    <row r="18" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G17" s="36"/>
+    </row>
+    <row r="18" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="27" t="s">
         <v>49</v>
       </c>
       <c r="C18" s="27"/>
       <c r="D18" s="27"/>
-      <c r="E18" s="35" t="s">
+      <c r="E18" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-    </row>
-    <row r="19" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+    </row>
+    <row r="19" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="26" t="s">
         <v>17</v>
       </c>
@@ -1031,7 +1031,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="16"/>
     </row>
-    <row r="20" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
         <v>8</v>
       </c>
@@ -1039,7 +1039,7 @@
       <c r="F20" s="16"/>
       <c r="G20" s="16"/>
     </row>
-    <row r="21" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
         <v>9</v>
       </c>
@@ -1047,7 +1047,7 @@
       <c r="F21" s="16"/>
       <c r="G21" s="16"/>
     </row>
-    <row r="22" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
         <v>10</v>
       </c>
@@ -1055,7 +1055,7 @@
       <c r="F22" s="16"/>
       <c r="G22" s="16"/>
     </row>
-    <row r="23" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
         <v>45</v>
       </c>
@@ -1063,7 +1063,7 @@
       <c r="F23" s="16"/>
       <c r="G23" s="16"/>
     </row>
-    <row r="24" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
         <v>27</v>
       </c>
@@ -1071,7 +1071,7 @@
       <c r="F24" s="16"/>
       <c r="G24" s="18"/>
     </row>
-    <row r="25" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="15" t="s">
         <v>46</v>
       </c>
@@ -1079,39 +1079,39 @@
       <c r="F25" s="27"/>
       <c r="G25" s="28"/>
     </row>
-    <row r="26" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="2:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="2:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="2:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="2:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="2:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="2:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="2:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="2:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="2:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="2:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="2:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="2:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="2:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="2:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="2:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="2:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="21" t="s">
         <v>12</v>
       </c>
@@ -1131,7 +1131,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="22"/>
       <c r="C55" s="22"/>
       <c r="D55" s="22"/>
@@ -1139,36 +1139,36 @@
       <c r="F55" s="23"/>
       <c r="G55" s="22"/>
     </row>
-    <row r="56" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="31" t="s">
+    <row r="56" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B56" s="31"/>
-      <c r="C56" s="31"/>
-      <c r="D56" s="31"/>
-      <c r="E56" s="31"/>
-      <c r="F56" s="31"/>
-      <c r="G56" s="31"/>
-      <c r="H56" s="31"/>
-      <c r="I56" s="31"/>
-      <c r="J56" s="31"/>
-      <c r="K56" s="31"/>
-    </row>
-    <row r="57" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="37"/>
+      <c r="C56" s="37"/>
+      <c r="D56" s="37"/>
+      <c r="E56" s="37"/>
+      <c r="F56" s="37"/>
+      <c r="G56" s="37"/>
+      <c r="H56" s="37"/>
+      <c r="I56" s="37"/>
+      <c r="J56" s="37"/>
+      <c r="K56" s="37"/>
+    </row>
+    <row r="57" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="63" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="65" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="66" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="67" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B67" s="21" t="s">
         <v>30</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="68" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B68" s="24"/>
       <c r="C68" s="24"/>
       <c r="D68" s="25"/>
@@ -1200,21 +1200,21 @@
       <c r="G68" s="24"/>
       <c r="H68" s="24"/>
     </row>
-    <row r="69" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="70" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="71" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="72" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="73" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="74" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="75" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="76" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="77" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="78" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="79" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B79" s="21" t="s">
         <v>30</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="80" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B80" s="24"/>
       <c r="C80" s="24"/>
       <c r="D80" s="25"/>
@@ -1246,21 +1246,21 @@
       <c r="G80" s="24"/>
       <c r="H80" s="24"/>
     </row>
-    <row r="81" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="82" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="83" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="88" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="84" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="85" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="86" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="87" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="88" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="89" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="90" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="91" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B91" s="21" t="s">
         <v>30</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="92" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B92" s="24"/>
       <c r="C92" s="24"/>
       <c r="D92" s="25"/>
@@ -1292,21 +1292,21 @@
       <c r="G92" s="24"/>
       <c r="H92" s="24"/>
     </row>
-    <row r="93" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="94" spans="2:8" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B94" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="95" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" spans="2:8" s="17" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="99" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="100" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="101" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="102" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="103" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:8" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="96" spans="2:8" s="17" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="97" spans="2:8" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="98" spans="2:8" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="99" spans="2:8" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="100" spans="2:8" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="101" spans="2:8" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="102" spans="2:8" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="103" spans="2:8" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B103" s="21" t="s">
         <v>37</v>
       </c>
@@ -1325,7 +1325,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="104" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:8" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B104" s="24"/>
       <c r="C104" s="24"/>
       <c r="D104" s="24"/>
@@ -1334,21 +1334,21 @@
       <c r="G104" s="24"/>
       <c r="H104" s="24"/>
     </row>
-    <row r="105" spans="2:8" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:8" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="106" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B106" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="107" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="108" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="110" spans="2:8" s="17" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="113" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="114" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="115" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="108" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="109" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="110" spans="2:8" s="17" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="111" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="112" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="113" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="114" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="115" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B115" s="21" t="s">
         <v>36</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="116" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B116" s="24"/>
       <c r="C116" s="24"/>
       <c r="D116" s="24"/>
@@ -1374,21 +1374,21 @@
       <c r="G116" s="24"/>
       <c r="H116" s="24"/>
     </row>
-    <row r="117" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="118" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B118" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="119" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" spans="2:8" s="17" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="127" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="120" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="121" spans="2:8" s="17" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="122" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="123" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="124" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="125" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="126" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="127" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B127" s="21" t="s">
         <v>39</v>
       </c>
@@ -1407,7 +1407,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="128" spans="2:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B128" s="24"/>
       <c r="C128" s="24"/>
       <c r="D128" s="24"/>
@@ -1416,8 +1416,8 @@
       <c r="G128" s="24"/>
       <c r="H128" s="24"/>
     </row>
-    <row r="129" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="130" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="130" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="20" t="s">
         <v>43</v>
       </c>
@@ -1432,20 +1432,9 @@
       <c r="J130" s="20"/>
       <c r="K130" s="20"/>
     </row>
-    <row r="131" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="E16:G16"/>
     <mergeCell ref="A56:K56"/>
@@ -1458,6 +1447,17 @@
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="A14:K14"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="7.874015748031496E-2" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.19685039370078741"/>

</xml_diff>